<commit_message>
added casey and emma profiles
Added Casey and Emma Profiles. Updated Cameron bio text
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Cameron_Lefebvre/Author_form.xlsx
+++ b/website_content_creation/authors/Cameron_Lefebvre/Author_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Cameron_Lefebvre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_532FE10695BB40FEE5D3FCDF0BE103DE683F0CFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A3B91BB-3562-4AB7-BA8E-9094A5488617}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_532FE10695BB40FEE5D3FCDF0BE103DE683F0CFF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F2DC733-7268-4587-92A5-BC176EF62289}"/>
   <bookViews>
-    <workbookView xWindow="20790" yWindow="-13605" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14235" yWindow="-16395" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Bio</t>
   </si>
   <si>
-    <t>I finished my undegraduate degree at Laurentian Univerity study deer mice in Algonquin Provincial Park. Now I'm excited to make the move to aquatic ecosystems and to learn everything I can in this field!</t>
-  </si>
-  <si>
     <t>Academic Supervisor (for students)</t>
   </si>
   <si>
@@ -160,6 +157,15 @@
   </si>
   <si>
     <t>Visiting and Co-supervised Students</t>
+  </si>
+  <si>
+    <t>I finished my undergraduate degree at Laurentian University studying deer mice in Algonquin Provincial Park. Now I'm excited to make the move to aquatic ecosystems and to learn everything I can in this field! I am currently working on biodiversity in benthic stream ecosystems.</t>
+  </si>
+  <si>
+    <t>MSc Biology</t>
+  </si>
+  <si>
+    <t>current</t>
   </si>
 </sst>
 </file>
@@ -771,7 +777,7 @@
   <dimension ref="A1:C1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -869,78 +875,84 @@
         <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="C20" s="16">
         <v>2025</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
@@ -960,24 +972,24 @@
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="32"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>36</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1007,32 +1019,32 @@
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>